<commit_message>
navigation menu in progress
</commit_message>
<xml_diff>
--- a/planning.xlsx
+++ b/planning.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DIEGO\BECA PROGRAMATE\portfolio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCE7BE21-D6F1-4F81-911F-8BC81890B25F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8091FDB4-4F0C-4C84-BD5D-BB29E54380D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5730" yWindow="2535" windowWidth="7500" windowHeight="6000" xr2:uid="{34E53257-1AC3-4821-B02E-45648F08EAAF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{34E53257-1AC3-4821-B02E-45648F08EAAF}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -454,7 +454,7 @@
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
portfolio First version 05 oct 2021
</commit_message>
<xml_diff>
--- a/planning.xlsx
+++ b/planning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DIEGO\BECA PROGRAMATE\portfolio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8091FDB4-4F0C-4C84-BD5D-BB29E54380D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57C276F0-D295-4C73-B9CA-8FBC6616978A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{34E53257-1AC3-4821-B02E-45648F08EAAF}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
   <si>
     <t xml:space="preserve">Martes </t>
   </si>
@@ -51,9 +51,6 @@
     <t>HTML</t>
   </si>
   <si>
-    <t>CSS</t>
-  </si>
-  <si>
     <t>Despliegue de repositorio en internet</t>
   </si>
   <si>
@@ -72,19 +69,31 @@
     <t>sobre mi</t>
   </si>
   <si>
-    <t>sección</t>
-  </si>
-  <si>
     <t>footer</t>
   </si>
   <si>
     <t>Descripcion</t>
   </si>
   <si>
-    <t>Secciones adicionales opcionales</t>
-  </si>
-  <si>
     <t>Planning portfolio</t>
+  </si>
+  <si>
+    <t>email form</t>
+  </si>
+  <si>
+    <t>timeline</t>
+  </si>
+  <si>
+    <t>proyectos</t>
+  </si>
+  <si>
+    <t>seccion</t>
+  </si>
+  <si>
+    <t>maquetacion</t>
+  </si>
+  <si>
+    <t>deploy</t>
   </si>
 </sst>
 </file>
@@ -108,12 +117,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -128,13 +143,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -451,36 +471,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9AAF8B5-2023-40FE-AC02-419BA98C3D6B}">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C18" sqref="A1:C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="29.85546875" customWidth="1"/>
+    <col min="1" max="1" width="17.85546875" customWidth="1"/>
+    <col min="2" max="2" width="47.42578125" customWidth="1"/>
     <col min="3" max="3" width="23.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="s">
+      <c r="A2" s="4"/>
+      <c r="B2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C2" t="s">
-        <v>17</v>
+      <c r="C2" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
@@ -494,38 +516,40 @@
       <c r="B4" t="s">
         <v>6</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B5" s="1" t="s">
+      <c r="A5" s="4"/>
+      <c r="B5" s="5" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="B6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>15</v>
-      </c>
+      <c r="A7" s="2"/>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -535,46 +559,67 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-      <c r="B11" t="s">
+      <c r="A11" s="4"/>
+      <c r="B11" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="6"/>
+      <c r="B13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="4"/>
+      <c r="B14" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="2"/>
+      <c r="B16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="2"/>
+      <c r="B18" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B13" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B16" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
-        <v>9</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="A7:A11"/>
+  <mergeCells count="6">
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A17:A18"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A6:A10"/>
+    <mergeCell ref="A12:A13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>